<commit_message>
updating code, changing language in process
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>29041,56</t>
+          <t>29038,98</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -494,7 +494,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>82,53</t>
+          <t>82,52</t>
         </is>
       </c>
     </row>
@@ -572,12 +572,12 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>BITCOIN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>LITECOIN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
@@ -604,16 +604,8 @@
       <c r="H1" s="3" t="n"/>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="A2" s="3" t="inlineStr"/>
+      <c r="B2" s="3" t="inlineStr"/>
       <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
@@ -622,16 +614,8 @@
       <c r="H2" s="3" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>A2</t>
-        </is>
-      </c>
+      <c r="A3" s="3" t="inlineStr"/>
+      <c r="B3" s="3" t="inlineStr"/>
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>

</xml_diff>

<commit_message>
language changing improved, currency class added and remembering
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>29038,98</t>
+          <t>29031,44</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -494,14 +494,14 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>82,52</t>
+          <t>1831,15</t>
         </is>
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>29796,75</t>
+          <t>0,616699</t>
         </is>
       </c>
     </row>
@@ -572,17 +572,17 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>BITCOIN</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ETHEREUM</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -604,9 +604,21 @@
       <c r="H1" s="3" t="n"/>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="3" t="inlineStr"/>
-      <c r="B2" s="3" t="inlineStr"/>
-      <c r="C2" s="3" t="inlineStr"/>
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
@@ -614,9 +626,21 @@
       <c r="H2" s="3" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr"/>
-      <c r="B3" s="3" t="inlineStr"/>
-      <c r="C3" s="3" t="inlineStr"/>
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>

</xml_diff>

<commit_message>
udpte colour error name in modifycoin:
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>0,160977</t>
+          <t>0,224235</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -494,7 +494,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>1866,02</t>
+          <t>29860,91</t>
         </is>
       </c>
     </row>
@@ -577,17 +577,17 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>ETHEREUM</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LITECOIN</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>GAMESWIFT</t>
+          <t>MOVER</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
@@ -609,12 +609,12 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr"/>
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
@@ -628,15 +628,15 @@
     <row r="3" ht="15" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>A2</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>A2</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr"/>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
           <t>A1</t>

</xml_diff>

<commit_message>
fetching coins after changing xlsx file patched
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>0,224235</t>
+          <t>342,18</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -577,17 +577,17 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
+          <t>ETHEREUM</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>LITECOIN</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
           <t>-</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>LITECOIN</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>MOVER</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
@@ -609,17 +609,17 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr"/>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
       <c r="G2" s="3" t="n"/>
@@ -631,17 +631,17 @@
           <t>A1</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
           <t>A1</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
+      <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
       <c r="G3" s="3" t="n"/>
@@ -671,7 +671,7 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>1887,36</t>
+          <t>2,632075</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updating loading app, some performance changes
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -463,52 +463,40 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>342,18</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>1868,22</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>111,31</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>0,258755</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+          <t>0,627401</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="3" t="n"/>
+      <c r="D1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>29860,91</t>
+          <t>29466,8</t>
         </is>
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>0,616699</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+          <t>83,67</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="2">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>0,339243</t>
+          <t>0,221543</t>
         </is>
       </c>
     </row>
@@ -539,7 +527,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -567,19 +555,19 @@
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
+          <t>ETHEREUM</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
           <t>BITCOIN</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>ETHEREUM</t>
-        </is>
-      </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
           <t>LITECOIN</t>
@@ -592,7 +580,7 @@
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
@@ -620,8 +608,12 @@
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr"/>
-      <c r="E2" s="3" t="inlineStr"/>
-      <c r="F2" s="3" t="inlineStr"/>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="n"/>
       <c r="G2" s="3" t="n"/>
       <c r="H2" s="3" t="n"/>
     </row>
@@ -633,17 +625,21 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr"/>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
           <t>A1</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr"/>
-      <c r="E3" s="3" t="inlineStr"/>
-      <c r="F3" s="3" t="inlineStr"/>
+      <c r="F3" s="3" t="n"/>
       <c r="G3" s="3" t="n"/>
       <c r="H3" s="3" t="n"/>
     </row>
@@ -662,48 +658,48 @@
   </sheetPr>
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>2,632075</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+          <t>0,627851</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
           <t>0,775888</t>
         </is>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="12.8" customHeight="1" s="2">
       <c r="C3" s="3" t="inlineStr">
         <is>
           <t>1894,75</t>
         </is>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="12.8" customHeight="1" s="2">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>29942,99</t>
         </is>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="12.8" customHeight="1" s="2">
       <c r="A8" s="3" t="inlineStr">
         <is>
           <t>1890,35</t>
         </is>
       </c>
     </row>
-    <row r="45">
+    <row r="45" ht="12.8" customHeight="1" s="2">
       <c r="A45" s="3" t="inlineStr">
         <is>
           <t>94,53</t>
@@ -737,7 +733,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -765,23 +761,23 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="4">
+    <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>0,070110464899</t>
         </is>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="12.8" customHeight="1" s="2">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>0,339243</t>
         </is>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="12.8" customHeight="1" s="2">
       <c r="A6" s="3" t="inlineStr">
         <is>
           <t>0,357891</t>
@@ -815,9 +811,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>0,750889</t>
@@ -851,7 +847,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -879,9 +875,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="45">
+    <row r="45" ht="12.8" customHeight="1" s="2">
       <c r="A45" s="3" t="inlineStr">
         <is>
           <t>0,747834</t>
@@ -915,16 +911,16 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="3">
+    <row r="3" ht="12.8" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>0,72346</t>
         </is>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>0,072419696968</t>

</xml_diff>

<commit_message>
update suggestion coin names. and some small changes
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -463,16 +463,16 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>0,001705</t>
+          <t>1,56</t>
         </is>
       </c>
       <c r="B1" s="3" t="n"/>
@@ -482,7 +482,7 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>26388,38</t>
+          <t>0,005513</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -551,102 +551,46 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>ETHEREUM</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>BITCOIN</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>LITECOIN</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>MOVER</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>AMP</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
           <t>-</t>
         </is>
       </c>
+      <c r="C1" s="3" t="n"/>
+      <c r="D1" s="3" t="n"/>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
       <c r="G1" s="3" t="n"/>
       <c r="H1" s="3" t="n"/>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="A2" s="3" t="inlineStr"/>
+      <c r="B2" s="3" t="inlineStr"/>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
       <c r="G2" s="3" t="n"/>
       <c r="H2" s="3" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>A2</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>A3</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
+      <c r="A3" s="3" t="inlineStr"/>
+      <c r="B3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
       <c r="G3" s="3" t="n"/>
       <c r="H3" s="3" t="n"/>
@@ -664,13 +608,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
@@ -683,6 +627,11 @@
       <c r="A2" s="3" t="inlineStr">
         <is>
           <t>0,775888</t>
+        </is>
+      </c>
+      <c r="S2" s="3" t="inlineStr">
+        <is>
+          <t>0,146</t>
         </is>
       </c>
     </row>
@@ -741,7 +690,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -769,7 +718,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
@@ -819,7 +768,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
@@ -855,7 +804,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -883,7 +832,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="45" ht="12.8" customHeight="1" s="2">
       <c r="A45" s="3" t="inlineStr">
@@ -919,7 +868,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="3" ht="12.8" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">

</xml_diff>

<commit_message>
added currency choice separatly for each asset
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>1,56</t>
+          <t>1592,56</t>
         </is>
       </c>
       <c r="B1" s="3" t="n"/>
@@ -482,7 +482,7 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>0,005513</t>
+          <t>1593,64</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update modify and add asset, gbp, eur added, each asset has unique currency to save
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -461,18 +461,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>1592,56</t>
+          <t>25093,43</t>
         </is>
       </c>
       <c r="B1" s="3" t="n"/>
@@ -482,7 +482,7 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>1593,64</t>
+          <t>2,203865</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,14 @@
     <row r="5" ht="12.8" customHeight="1" s="2">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>0,221543</t>
+          <t>897,93</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="12.8" customHeight="1" s="2">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>1592,24</t>
         </is>
       </c>
     </row>
@@ -527,7 +534,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -549,25 +556,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+          <t>bitcoin</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="n"/>
       <c r="C1" s="3" t="n"/>
       <c r="D1" s="3" t="n"/>
       <c r="E1" s="3" t="n"/>
@@ -576,8 +579,12 @@
       <c r="H1" s="3" t="n"/>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="3" t="inlineStr"/>
-      <c r="B2" s="3" t="inlineStr"/>
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n"/>
       <c r="C2" s="3" t="n"/>
       <c r="D2" s="3" t="n"/>
       <c r="E2" s="3" t="n"/>
@@ -586,14 +593,28 @@
       <c r="H2" s="3" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr"/>
-      <c r="B3" s="3" t="inlineStr"/>
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n"/>
       <c r="C3" s="3" t="n"/>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
       <c r="G3" s="3" t="n"/>
       <c r="H3" s="3" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="2">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n"/>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="3" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -614,12 +635,12 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>0,627851</t>
+          <t>1592,24</t>
         </is>
       </c>
     </row>
@@ -636,9 +657,21 @@
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="2">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>114902,49</t>
+        </is>
+      </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
           <t>1894,75</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="2">
+      <c r="S5" s="3" t="inlineStr">
+        <is>
+          <t>0,137275</t>
         </is>
       </c>
     </row>
@@ -690,7 +723,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -718,7 +751,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
@@ -768,7 +801,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
@@ -804,7 +837,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -832,7 +865,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="45" ht="12.8" customHeight="1" s="2">
       <c r="A45" s="3" t="inlineStr">
@@ -868,7 +901,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="3" ht="12.8" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">

</xml_diff>

<commit_message>
update etf metal price added, some features improved
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -574,7 +574,7 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>bitcoin</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -594,11 +594,7 @@
       <c r="H1" s="3" t="n"/>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="A2" s="3" t="inlineStr"/>
       <c r="B2" s="3" t="inlineStr"/>
       <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="n"/>
@@ -608,11 +604,7 @@
       <c r="H2" s="3" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
+      <c r="A3" s="3" t="inlineStr"/>
       <c r="B3" s="3" t="inlineStr"/>
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="n"/>

</xml_diff>